<commit_message>
Readme formatting; WEMI table
</commit_message>
<xml_diff>
--- a/relationship_mapping.xlsx
+++ b/relationship_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kek67197.MYID\AppData\Roaming\OCLC\Connex\Macros\Projects\RelationshipLabels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4CED73-6B00-41CB-850D-8C8723C72C7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D5D718-4418-472E-AAB4-FBD284D28433}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="2" xr2:uid="{88E9D25B-84E2-4D1B-9CF6-0F03DEA062E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{88E9D25B-84E2-4D1B-9CF6-0F03DEA062E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Agents" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="1529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="1555">
   <si>
     <t>creator</t>
   </si>
@@ -3971,9 +3971,6 @@
     <t>abridgement of</t>
   </si>
   <si>
-    <t>absorebed by</t>
-  </si>
-  <si>
     <t>absorbed in part by</t>
   </si>
   <si>
@@ -4544,9 +4541,6 @@
     <t>related expression of</t>
   </si>
   <si>
-    <t>expression of</t>
-  </si>
-  <si>
     <t>representative expression</t>
   </si>
   <si>
@@ -4556,18 +4550,12 @@
     <t>related work</t>
   </si>
   <si>
-    <t>analysied in</t>
-  </si>
-  <si>
     <t>representative expression of</t>
   </si>
   <si>
     <t>work expressed</t>
   </si>
   <si>
-    <t>Shouldn't this just be "expression"? "Is expression of" would need an expression as its subject and work as its object.</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -4614,6 +4602,96 @@
   </si>
   <si>
     <t>onscreen presenter</t>
+  </si>
+  <si>
+    <t>[Expression to Expression]</t>
+  </si>
+  <si>
+    <t>related expression</t>
+  </si>
+  <si>
+    <t>absorbed by</t>
+  </si>
+  <si>
+    <t>absorption of</t>
+  </si>
+  <si>
+    <t>abstracted as</t>
+  </si>
+  <si>
+    <t>adapted as</t>
+  </si>
+  <si>
+    <t>aggregated by</t>
+  </si>
+  <si>
+    <t>aggregates</t>
+  </si>
+  <si>
+    <t>appendix</t>
+  </si>
+  <si>
+    <t>arranged as</t>
+  </si>
+  <si>
+    <t>arrangement of</t>
+  </si>
+  <si>
+    <t>augmentation of</t>
+  </si>
+  <si>
+    <t>deriviative expression</t>
+  </si>
+  <si>
+    <t>dubbed version</t>
+  </si>
+  <si>
+    <t>dubbed version of</t>
+  </si>
+  <si>
+    <t>errata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expanded as </t>
+  </si>
+  <si>
+    <t>merger of</t>
+  </si>
+  <si>
+    <t>merged to form</t>
+  </si>
+  <si>
+    <t>revised as</t>
+  </si>
+  <si>
+    <t>revision of</t>
+  </si>
+  <si>
+    <t>screenplay for video</t>
+  </si>
+  <si>
+    <t>supplement</t>
+  </si>
+  <si>
+    <t>translated as</t>
+  </si>
+  <si>
+    <t>translation of</t>
+  </si>
+  <si>
+    <t>expression of [Shouldn't this just be "expression"? "Is expression of" would need an expression as its subject and work as its object.]</t>
+  </si>
+  <si>
+    <t>WWIRI</t>
+  </si>
+  <si>
+    <t>WEIRI</t>
+  </si>
+  <si>
+    <t>EWIRI</t>
+  </si>
+  <si>
+    <t>EEIRI</t>
   </si>
 </sst>
 </file>
@@ -9834,1110 +9912,1588 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F12BAC-9A30-4305-86EA-C3B11800714B}">
-  <dimension ref="A1:I219"/>
+  <dimension ref="A1:H219"/>
   <sheetViews>
-    <sheetView topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="I205" sqref="I205"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1311</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1312</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>1313</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>1314</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B9" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B10" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>1316</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B12" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>1317</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B14" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B15" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>1319</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B16" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B18" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>1321</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B19" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>1322</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B20" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>1323</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B21" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>1324</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B22" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B23" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>1326</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B24" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>1327</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B25" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>1328</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B26" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>1329</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B27" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>1330</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B28" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B29" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>1332</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B30" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B31" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>1335</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B33" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>1336</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B34" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>1337</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B35" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>1338</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B37" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>1340</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C41" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>1341</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B43" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>1342</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B46" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>1343</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B47" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>1344</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B48" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>1345</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B49" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>1346</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B50" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>1347</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>1348</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>1349</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B53" t="s">
         <v>1350</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>1351</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B55" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>1352</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>1353</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B57" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>1354</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>1355</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>1356</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C61" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>1357</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B62" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>1358</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B64" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>1360</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B65" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>1361</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B66" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>1362</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="C68" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>1363</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1499</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>1364</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B73" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>1365</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B74" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>1366</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B75" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>1367</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B76" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>1368</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B80" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>1369</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="C82" t="s">
         <v>1369</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>1370</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="B83" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B84" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="B87" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>1374</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B88" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="B89" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>1376</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B90" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>1377</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>1378</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="B92" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="B94" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>1381</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="B95" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="B96" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>1383</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="B98" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>1386</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B100" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B101" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>1388</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="B102" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>1389</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>1390</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>1391</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>1392</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>1393</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>1394</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>1395</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="B109" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>1396</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>1397</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="B111" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>1398</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>1399</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>1400</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="B114" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>1401</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="B115" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>1402</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="B116" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>1403</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="B117" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>1404</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B118" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B119" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>1406</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B120" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>1407</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B123" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>1408</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B124" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>1409</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B125" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>1410</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="B126" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>1413</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="B127" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>1414</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="B128" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>1415</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="B129" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>1416</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="B130" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>1417</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="B131" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>1418</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="B132" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>1419</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="B133" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>1420</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="B134" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>1421</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="B135" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>1422</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>1423</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="B137" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>1424</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="B138" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="B139" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>1426</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="B140" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>1427</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="B141" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>1428</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="B142" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>1429</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="B143" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>1430</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>1431</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>1432</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="B146" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>1433</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="B147" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>1434</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="B148" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>1435</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="B149" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>1436</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="B150" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>1437</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="B151" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D154" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>1438</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="C155" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>1439</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="B159" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>1440</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="B161" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>1441</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="B162" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>1442</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>1443</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="B163" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>1445</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="B164" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>1446</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="B165" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>1447</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="B166" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>1448</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="B167" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>1449</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>1450</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>1451</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>1452</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="B172" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>1454</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>1455</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>1456</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>1457</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>1458</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="B177" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>1459</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="B178" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>1460</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>1461</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>1462</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>1463</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>66</v>
+      </c>
+      <c r="C183" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>1464</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="D184" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>1465</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>1466</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>1467</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="B187" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>1468</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="B188" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>1469</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="B189" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B190" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>1470</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="B191" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>1471</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="B192" t="s">
         <v>1471</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="B193" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>1473</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="B194" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>1474</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="B195" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>1475</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
         <v>1476</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>1477</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>1478</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>1479</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>1480</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>1481</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>1482</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>1483</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>1484</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>1485</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>1486</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>1487</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>1488</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>1489</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="B212" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>1490</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="B213" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>1491</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="B214" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>1492</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>1493</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="B216" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>1494</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="B217" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>1495</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>1496</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>1497</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>1498</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>1499</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>1502</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>1503</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>1504</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>1505</v>
-      </c>
-      <c r="I205" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>1506</v>
-      </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>1439</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>1507</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+      <c r="B218" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D219" t="s">
         <v>1508</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>1509</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>1498</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>1499</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>1502</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>1511</v>
       </c>
     </row>
   </sheetData>
@@ -10949,7 +11505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A70CA9A-5FF9-4E86-A663-A58967A4F044}">
   <dimension ref="A1:D302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+    <sheetView topLeftCell="A171" workbookViewId="0">
       <selection activeCell="C191" sqref="C191"/>
     </sheetView>
   </sheetViews>
@@ -10963,13 +11519,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1513</v>
+        <v>1509</v>
       </c>
       <c r="B1" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
       <c r="C1" t="s">
-        <v>1515</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10991,7 +11547,7 @@
         <v>713</v>
       </c>
       <c r="C3" t="s">
-        <v>1516</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -11027,7 +11583,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>1517</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -11038,7 +11594,7 @@
         <v>721</v>
       </c>
       <c r="C7" t="s">
-        <v>1521</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -11049,7 +11605,7 @@
         <v>723</v>
       </c>
       <c r="C8" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -11212,7 +11768,7 @@
         <v>757</v>
       </c>
       <c r="C25" t="s">
-        <v>1519</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -11223,7 +11779,7 @@
         <v>759</v>
       </c>
       <c r="C26" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -11245,7 +11801,7 @@
         <v>763</v>
       </c>
       <c r="C28" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -11526,7 +12082,7 @@
         <v>826</v>
       </c>
       <c r="C60" t="s">
-        <v>1523</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -11537,7 +12093,7 @@
         <v>828</v>
       </c>
       <c r="C61" t="s">
-        <v>1524</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -12164,7 +12720,7 @@
         <v>977</v>
       </c>
       <c r="C136" t="s">
-        <v>1525</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -12455,7 +13011,7 @@
         <v>1041</v>
       </c>
       <c r="C169" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -12573,7 +13129,7 @@
         <v>1069</v>
       </c>
       <c r="C183" t="s">
-        <v>1527</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -12646,7 +13202,7 @@
         <v>1085</v>
       </c>
       <c r="C191" t="s">
-        <v>1528</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -13164,7 +13720,7 @@
         <v>1207</v>
       </c>
       <c r="C252" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -13600,16 +14156,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="36354d7e-163f-40eb-b978-cce71771c1f1" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -13618,7 +14164,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004222493D04F36E498343FD1F263FE457" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dff6174afa9775cdde48c5192d5c745c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="36354d7e-163f-40eb-b978-cce71771c1f1" xmlns:ns4="14a80677-60f4-4cc2-8127-0186e2cf64a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7e071efaea11a250735ad30ec12af2e" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13882,25 +14428,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C82FB17-50E6-4BA2-9476-82AA38D7CF00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="14a80677-60f4-4cc2-8127-0186e2cf64a5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="36354d7e-163f-40eb-b978-cce71771c1f1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="36354d7e-163f-40eb-b978-cce71771c1f1" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B72B49D-CCC7-45F7-8526-1F385CB54990}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -13908,7 +14446,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CCA7AF7-7753-432F-91DC-8CC84E5DC301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13926,4 +14464,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C82FB17-50E6-4BA2-9476-82AA38D7CF00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="14a80677-60f4-4cc2-8127-0186e2cf64a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="36354d7e-163f-40eb-b978-cce71771c1f1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Refactor, outline batch mode
</commit_message>
<xml_diff>
--- a/relationship_mapping.xlsx
+++ b/relationship_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kek67197.MYID\AppData\Roaming\OCLC\Connex\Macros\Projects\RelationshipLabels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D5D718-4418-472E-AAB4-FBD284D28433}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FA6977-E4E0-4A13-84FE-94A0DED8029D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{88E9D25B-84E2-4D1B-9CF6-0F03DEA062E6}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="1555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="1581">
   <si>
     <t>creator</t>
   </si>
@@ -4692,6 +4692,84 @@
   </si>
   <si>
     <t>EEIRI</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10198</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10167</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10125</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10145</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10146</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10225</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10224</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10126</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10107</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10089</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10193</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10142</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10155</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10091</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10248</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10247</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10251</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10252</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10113</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10189</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10165</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10030</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10094</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10025</t>
+  </si>
+  <si>
+    <t>http://rdaregistry.info/Elements/w/P10235</t>
   </si>
 </sst>
 </file>
@@ -4715,15 +4793,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -4731,15 +4815,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9915,1588 +10017,1708 @@
   <dimension ref="A1:H219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="4" width="31.5703125" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="4" width="31.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41" style="3" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="27" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1310</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1525</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1502</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>1505</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1551</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>1552</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>1553</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>1554</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1526</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>1577</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>1506</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>1577</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>1311</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>1555</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>1503</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>1577</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>1312</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>1312</v>
       </c>
+      <c r="E6" s="5" t="s">
+        <v>1556</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>1313</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>1313</v>
       </c>
+      <c r="E7" s="5" t="s">
+        <v>1557</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>1527</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>1527</v>
       </c>
+      <c r="E8" s="5" t="s">
+        <v>1558</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>1314</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>1314</v>
       </c>
+      <c r="E9" s="5" t="s">
+        <v>1559</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>1315</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="4" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>1528</v>
+      <c r="E11" s="5" t="s">
+        <v>1560</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>1316</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>1316</v>
       </c>
+      <c r="E12" s="5" t="s">
+        <v>1562</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="A13" s="3" t="s">
         <v>1529</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>1529</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>1563</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>1317</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>1317</v>
       </c>
+      <c r="E14" s="5" t="s">
+        <v>1564</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>1318</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>1318</v>
       </c>
+      <c r="E15" s="5" t="s">
+        <v>1565</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>1319</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>1319</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="E16" s="5" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>1530</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B17" s="4" t="s">
+        <v>1530</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>1320</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E18" s="5" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>1321</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>1321</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E19" s="5" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>1322</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>1322</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="E20" s="5" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>1323</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>1323</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E21" s="5" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>1324</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>1324</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="E22" s="5" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>1325</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="E23" s="5" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>1326</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>1326</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>1327</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>1327</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>1328</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>1329</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>1330</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>1330</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>1331</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>1331</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>1332</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>1332</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>1333</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>1333</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>1334</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>1335</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>1335</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>1336</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>1336</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="3" t="s">
         <v>1337</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>1337</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>1339</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>1339</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>1338</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>1338</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>1531</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>1532</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="3" t="s">
         <v>1496</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="4" t="s">
         <v>1496</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="3" t="s">
         <v>1340</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="4" t="s">
         <v>1340</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="B42" s="4" t="s">
         <v>1533</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>1341</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>1341</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>1534</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="B45" s="4" t="s">
         <v>1535</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="3" t="s">
         <v>1342</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>1536</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="3" t="s">
         <v>1343</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="4" t="s">
         <v>1343</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>1344</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>1344</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>1345</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="4" t="s">
         <v>1345</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>1346</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="4" t="s">
         <v>1346</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>1347</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>1348</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>1349</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="4" t="s">
         <v>1350</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>1350</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="4" t="s">
         <v>1349</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>1351</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="4" t="s">
         <v>1351</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>1353</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="4" t="s">
         <v>1353</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="E56" s="5" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>1352</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="4" t="s">
         <v>1352</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="E57" s="5" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>1354</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>1355</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>1497</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="4" t="s">
         <v>1497</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>1356</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="4" t="s">
         <v>1356</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>1357</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="4" t="s">
         <v>1357</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>1359</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="4" t="s">
         <v>1359</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>1358</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="4" t="s">
         <v>1358</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="3" t="s">
         <v>1360</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="4" t="s">
         <v>1360</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="3" t="s">
         <v>1361</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>1361</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="3" t="s">
         <v>1498</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="4" t="s">
         <v>1498</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="3" t="s">
         <v>1362</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="4" t="s">
         <v>1362</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="3" t="s">
         <v>1363</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+      <c r="B70" s="4" t="s">
         <v>1537</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="3" t="s">
         <v>1499</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="4" t="s">
         <v>1499</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="3" t="s">
         <v>1364</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="4" t="s">
         <v>1364</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="3" t="s">
         <v>1365</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="4" t="s">
         <v>1365</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="3" t="s">
         <v>1366</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="4" t="s">
         <v>1366</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="3" t="s">
         <v>1367</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="4" t="s">
         <v>1367</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+      <c r="B77" s="4" t="s">
         <v>1538</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+      <c r="B78" s="4" t="s">
         <v>1539</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="3" t="s">
         <v>1540</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="4" t="s">
         <v>1540</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="3" t="s">
         <v>1368</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="4" t="s">
         <v>1368</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>1500</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="4" t="s">
         <v>1500</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>1369</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="4" t="s">
         <v>1369</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>1370</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="4" t="s">
         <v>1541</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>1371</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="4" t="s">
         <v>1371</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C85" s="4" t="s">
         <v>1550</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>1373</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="4" t="s">
         <v>1373</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>1372</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="4" t="s">
         <v>1372</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>1374</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="4" t="s">
         <v>1374</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>1375</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="4" t="s">
         <v>1375</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>1376</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="4" t="s">
         <v>1376</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="E90" s="5" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>1378</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="4" t="s">
         <v>1378</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>1377</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="4" t="s">
         <v>1377</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>1380</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="4" t="s">
         <v>1380</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>1379</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="4" t="s">
         <v>1379</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>1381</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="4" t="s">
         <v>1381</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
         <v>1382</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="4" t="s">
         <v>1382</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>1384</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="4" t="s">
         <v>1384</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
         <v>1383</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="4" t="s">
         <v>1383</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>1386</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="4" t="s">
         <v>1386</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
         <v>1385</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="4" t="s">
         <v>1385</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
         <v>1387</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="4" t="s">
         <v>1387</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>1388</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="4" t="s">
         <v>1388</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
         <v>1389</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>1390</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>1391</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
         <v>1392</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>1393</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>1394</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>1395</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="4" t="s">
         <v>1395</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="E109" s="5" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>1397</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="4" t="s">
         <v>1397</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="E110" s="5" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>1396</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="4" t="s">
         <v>1396</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="E111" s="5" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>1398</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="3" t="s">
         <v>1399</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="3" t="s">
         <v>1400</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="4" t="s">
         <v>1543</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="3" t="s">
         <v>1401</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="4" t="s">
         <v>1542</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="3" t="s">
         <v>1402</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="4" t="s">
         <v>1402</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="3" t="s">
         <v>1403</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="4" t="s">
         <v>1403</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="3" t="s">
         <v>1404</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="4" t="s">
         <v>1404</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="3" t="s">
         <v>1405</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="4" t="s">
         <v>1405</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="3" t="s">
         <v>1406</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="4" t="s">
         <v>1406</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" s="3" t="s">
         <v>1412</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="4" t="s">
         <v>1412</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="3" t="s">
         <v>1411</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="4" t="s">
         <v>1411</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" s="3" t="s">
         <v>1407</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="4" t="s">
         <v>1407</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="A124" s="3" t="s">
         <v>1408</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="4" t="s">
         <v>1408</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" s="3" t="s">
         <v>1409</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="4" t="s">
         <v>1409</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="A126" s="3" t="s">
         <v>1410</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="4" t="s">
         <v>1410</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="A127" s="3" t="s">
         <v>1413</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="4" t="s">
         <v>1413</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="A128" s="3" t="s">
         <v>1414</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="4" t="s">
         <v>1414</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="3" t="s">
         <v>1415</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="4" t="s">
         <v>1415</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="A130" s="3" t="s">
         <v>1416</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="4" t="s">
         <v>1416</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" s="3" t="s">
         <v>1417</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="4" t="s">
         <v>1417</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" s="3" t="s">
         <v>1418</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="4" t="s">
         <v>1418</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="3" t="s">
         <v>1419</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="4" t="s">
         <v>1419</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" s="3" t="s">
         <v>1420</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="4" t="s">
         <v>1420</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="3" t="s">
         <v>1421</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="4" t="s">
         <v>1421</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="A136" s="3" t="s">
         <v>1423</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="4" t="s">
         <v>1423</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A137" s="3" t="s">
         <v>1422</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="4" t="s">
         <v>1422</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="A138" s="3" t="s">
         <v>1424</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="4" t="s">
         <v>1424</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="A139" s="3" t="s">
         <v>1425</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="4" t="s">
         <v>1425</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="A140" s="3" t="s">
         <v>1426</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="4" t="s">
         <v>1426</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="A141" s="3" t="s">
         <v>1427</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="4" t="s">
         <v>1427</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="A142" s="3" t="s">
         <v>1428</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="4" t="s">
         <v>1428</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="A143" s="3" t="s">
         <v>1429</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="4" t="s">
         <v>1429</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="A144" s="3" t="s">
         <v>1430</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="A145" s="3" t="s">
         <v>1431</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="A146" s="3" t="s">
         <v>1432</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="4" t="s">
         <v>1432</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="A147" s="3" t="s">
         <v>1433</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="4" t="s">
         <v>1433</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="A148" s="3" t="s">
         <v>1434</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="4" t="s">
         <v>1434</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="A149" s="3" t="s">
         <v>1435</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="4" t="s">
         <v>1435</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="A150" s="3" t="s">
         <v>1436</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="4" t="s">
         <v>1436</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="A151" s="3" t="s">
         <v>1437</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="4" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C152" t="s">
+      <c r="C152" s="4" t="s">
         <v>1504</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D153" t="s">
+      <c r="D153" s="4" t="s">
         <v>1507</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="A154" s="3" t="s">
         <v>1501</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="4" t="s">
         <v>1501</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="A155" s="3" t="s">
         <v>1438</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="4" t="s">
         <v>1438</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
+      <c r="B156" s="4" t="s">
         <v>1544</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" t="s">
+      <c r="B157" s="4" t="s">
         <v>1545</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="A158" s="3" t="s">
         <v>1444</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="4" t="s">
         <v>1444</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="A159" s="3" t="s">
         <v>1439</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="4" t="s">
         <v>1439</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="A160" s="3" t="s">
         <v>1443</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="4" t="s">
         <v>1443</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="A161" s="3" t="s">
         <v>1440</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="4" t="s">
         <v>1440</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="A162" s="3" t="s">
         <v>1441</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="4" t="s">
         <v>1441</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="A163" s="3" t="s">
         <v>1442</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="4" t="s">
         <v>1546</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="A164" s="3" t="s">
         <v>1445</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="4" t="s">
         <v>1445</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="A165" s="3" t="s">
         <v>1446</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="4" t="s">
         <v>1446</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="A166" s="3" t="s">
         <v>1447</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="4" t="s">
         <v>1447</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="A167" s="3" t="s">
         <v>1448</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="4" t="s">
         <v>1448</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="A168" s="3" t="s">
         <v>1449</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="A169" s="3" t="s">
         <v>1450</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="A170" s="3" t="s">
         <v>1451</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="A171" s="3" t="s">
         <v>1452</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="A172" s="3" t="s">
         <v>1453</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="4" t="s">
         <v>1453</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="A173" s="3" t="s">
         <v>1454</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="A174" s="3" t="s">
         <v>1455</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="A175" s="3" t="s">
         <v>1456</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="A176" s="3" t="s">
         <v>1457</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="A177" s="3" t="s">
         <v>1458</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="4" t="s">
         <v>1458</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+      <c r="A178" s="3" t="s">
         <v>1459</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="4" t="s">
         <v>1459</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+      <c r="A179" s="3" t="s">
         <v>1460</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+      <c r="A180" s="3" t="s">
         <v>1461</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+      <c r="A181" s="3" t="s">
         <v>1462</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="A182" s="3" t="s">
         <v>1463</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="A183" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="A184" s="3" t="s">
         <v>1464</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="4" t="s">
         <v>1464</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="A185" s="3" t="s">
         <v>1465</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="A186" s="3" t="s">
         <v>1466</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="A187" s="3" t="s">
         <v>1467</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="4" t="s">
         <v>1467</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="A188" s="3" t="s">
         <v>1468</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="4" t="s">
         <v>1468</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="A189" s="3" t="s">
         <v>1469</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="4" t="s">
         <v>1469</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="A190" s="3" t="s">
         <v>1547</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="4" t="s">
         <v>1547</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="A191" s="3" t="s">
         <v>1470</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="4" t="s">
         <v>1470</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="A192" s="3" t="s">
         <v>1471</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="4" t="s">
         <v>1471</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="A193" s="3" t="s">
         <v>1472</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="4" t="s">
         <v>1472</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="A194" s="3" t="s">
         <v>1473</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="4" t="s">
         <v>1473</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="A195" s="3" t="s">
         <v>1474</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="4" t="s">
         <v>1474</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="A196" s="3" t="s">
         <v>1475</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="A197" s="3" t="s">
         <v>1476</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+      <c r="A198" s="3" t="s">
         <v>1477</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="A199" s="3" t="s">
         <v>1478</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+      <c r="A200" s="3" t="s">
         <v>1479</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+      <c r="A201" s="3" t="s">
         <v>1480</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+      <c r="A202" s="3" t="s">
         <v>1481</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+      <c r="A203" s="3" t="s">
         <v>1482</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+      <c r="A204" s="3" t="s">
         <v>1483</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+      <c r="A205" s="3" t="s">
         <v>1484</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+      <c r="A206" s="3" t="s">
         <v>1485</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+      <c r="A207" s="3" t="s">
         <v>1486</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+      <c r="A208" s="3" t="s">
         <v>1487</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="A209" s="3" t="s">
         <v>1488</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
+      <c r="B210" s="4" t="s">
         <v>1548</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
+      <c r="B211" s="4" t="s">
         <v>1549</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+      <c r="A212" s="3" t="s">
         <v>1489</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="4" t="s">
         <v>1489</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+      <c r="A213" s="3" t="s">
         <v>1490</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="4" t="s">
         <v>1490</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="A214" s="3" t="s">
         <v>1491</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="4" t="s">
         <v>1491</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="A215" s="3" t="s">
         <v>1492</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="A216" s="3" t="s">
         <v>1493</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="4" t="s">
         <v>1493</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="A217" s="3" t="s">
         <v>1494</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="4" t="s">
         <v>1494</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+      <c r="A218" s="3" t="s">
         <v>1495</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" s="4" t="s">
         <v>1495</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D219" t="s">
+      <c r="D219" s="4" t="s">
         <v>1508</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{D5AF80DA-4387-4060-A430-4075588ECA14}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{C34AF7F3-829A-4687-A84D-9F3762525B2F}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{B4FF9EE0-362C-4EB3-8A29-3AFBF393EA6F}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{9890F2EE-20DD-4F84-9D98-27064FA964E8}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{F8ECB718-D70C-4576-B25D-BBF5A7904048}"/>
+    <hyperlink ref="E11" r:id="rId6" xr:uid="{FDA893EB-F98E-486F-81DD-CD835E0E5154}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{1AE52540-FEF7-4D27-AC87-110524FAC7EA}"/>
+    <hyperlink ref="E12" r:id="rId8" xr:uid="{FED2BEC0-53F2-4E41-BFB9-29417555EC70}"/>
+    <hyperlink ref="E13" r:id="rId9" xr:uid="{D9E8FA51-AF4B-4D5E-8248-A7F3BB0EDF79}"/>
+    <hyperlink ref="E14" r:id="rId10" xr:uid="{9DC1CDA6-BA00-4FDD-AE79-168298A38EE3}"/>
+    <hyperlink ref="E15" r:id="rId11" xr:uid="{C1E599EE-1872-404B-869B-692F847FD267}"/>
+    <hyperlink ref="E16" r:id="rId12" xr:uid="{88D67083-85C0-4617-BEB3-78A595BEFC59}"/>
+    <hyperlink ref="E17" r:id="rId13" xr:uid="{2BBE021C-0DB4-47C7-8B76-1CC316F9FD66}"/>
+    <hyperlink ref="E18" r:id="rId14" xr:uid="{D40D98F8-4006-4913-91CD-F4D0E832AC9E}"/>
+    <hyperlink ref="E57" r:id="rId15" xr:uid="{8FBD1EB8-C956-425F-BB9C-02781B82E52C}"/>
+    <hyperlink ref="E56" r:id="rId16" xr:uid="{E1B9EF86-E6FC-4CA8-9162-8F17B47144FE}"/>
+    <hyperlink ref="E19" r:id="rId17" xr:uid="{3174D9D3-D61A-458D-AA0B-E0B755E08C68}"/>
+    <hyperlink ref="E90" r:id="rId18" xr:uid="{85325F41-2531-4560-A887-CF0FBDBD4828}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{91F9AD0C-2A13-4C75-A60B-401AB9646680}"/>
+    <hyperlink ref="E109" r:id="rId20" xr:uid="{6BB6D37C-C092-4B31-B17C-241324CFAC28}"/>
+    <hyperlink ref="E110" r:id="rId21" xr:uid="{9F15AA92-91CA-4C5A-9ED1-573698C6989D}"/>
+    <hyperlink ref="E111" r:id="rId22" xr:uid="{787EB579-79EA-4D42-A568-7D5D11BD468F}"/>
+    <hyperlink ref="E21" r:id="rId23" xr:uid="{1AA10442-65F0-4CAE-84FC-94DF1C279FA4}"/>
+    <hyperlink ref="E22" r:id="rId24" xr:uid="{2C47BD6C-B33A-42A3-AA97-7DF4ABDABE7B}"/>
+    <hyperlink ref="E23" r:id="rId25" xr:uid="{5E1352AD-9C87-4F58-A125-61275ECA11E6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14165,6 +14387,16 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="36354d7e-163f-40eb-b978-cce71771c1f1" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004222493D04F36E498343FD1F263FE457" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dff6174afa9775cdde48c5192d5c745c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="36354d7e-163f-40eb-b978-cce71771c1f1" xmlns:ns4="14a80677-60f4-4cc2-8127-0186e2cf64a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7e071efaea11a250735ad30ec12af2e" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14428,16 +14660,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="36354d7e-163f-40eb-b978-cce71771c1f1" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B72B49D-CCC7-45F7-8526-1F385CB54990}">
   <ds:schemaRefs>
@@ -14447,6 +14669,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C82FB17-50E6-4BA2-9476-82AA38D7CF00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="14a80677-60f4-4cc2-8127-0186e2cf64a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="36354d7e-163f-40eb-b978-cce71771c1f1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CCA7AF7-7753-432F-91DC-8CC84E5DC301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14464,22 +14704,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C82FB17-50E6-4BA2-9476-82AA38D7CF00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="14a80677-60f4-4cc2-8127-0186e2cf64a5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="36354d7e-163f-40eb-b978-cce71771c1f1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>